<commit_message>
modified parameters for nvenc
</commit_message>
<xml_diff>
--- a/Encodings Speed Trial 1.xlsx
+++ b/Encodings Speed Trial 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmad\Documents\video_compression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25058989-361B-49CB-B63B-E8822730597D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533C360F-EAF2-4BD8-B6E6-CBC906ED5E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{5CC20662-CD28-4FF1-B3EE-7585E5D37CCE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{5CC20662-CD28-4FF1-B3EE-7585E5D37CCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="74">
   <si>
     <t>Codec</t>
   </si>
@@ -240,13 +240,34 @@
   </si>
   <si>
     <t>Encoding Speed</t>
+  </si>
+  <si>
+    <t>input_7.y4m</t>
+  </si>
+  <si>
+    <t>104876.8kbits/s</t>
+  </si>
+  <si>
+    <t>7767.9kbits/s</t>
+  </si>
+  <si>
+    <t>0.0393x</t>
+  </si>
+  <si>
+    <t>1.05x</t>
+  </si>
+  <si>
+    <t>1.06x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,16 +275,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -271,13 +306,107 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,1462 +741,1895 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA4C29D-0DA0-43B3-8DB7-8DFDB7445F1D}">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:Z50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.08984375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.6328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.90625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="22" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="14">
         <v>643</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="15">
         <v>7.45</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="16">
         <f>(D2/C2)</f>
         <v>1.1586314152410576E-2</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="13">
         <v>99.97</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="14">
         <v>3.78</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="13">
         <v>0.35</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="13">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="6">
         <v>643</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="7">
         <v>6</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="8">
         <f t="shared" ref="E3:E43" si="0">(D3/C3)</f>
         <v>9.3312597200622092E-3</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="5">
         <v>99.97</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="6">
         <v>1.61</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="5">
         <v>0.32</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="5">
         <v>27</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="10">
         <v>643</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="11">
         <v>3.33</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="12">
         <f t="shared" si="0"/>
         <v>5.1788491446345258E-3</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="9">
         <v>99.53</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="10">
         <v>6.64</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="9">
         <v>0.48</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="9">
         <v>3</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="Y4"/>
+      <c r="Z4"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>643</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="7">
         <v>6.17</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="8">
         <f t="shared" si="0"/>
         <v>9.5956454121306368E-3</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="5">
         <v>99.96</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="6">
         <v>1.92</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="5">
         <v>0.51</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="5">
         <v>11</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>643</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="7">
         <v>4.09</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="8">
         <f t="shared" si="0"/>
         <v>6.3608087091757389E-3</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="5">
         <v>99.97</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="6">
         <v>297.89999999999998</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="5">
         <v>0.81</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>643</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="7">
         <v>5.56</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="8">
         <f t="shared" si="0"/>
         <v>8.6469673405909792E-3</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="5">
         <v>99.98</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="6">
         <v>3.6</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="5">
         <v>0.69</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="5">
         <v>1</v>
       </c>
-      <c r="K7" t="s">
+      <c r="J7" s="5"/>
+      <c r="K7" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>643</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="7">
         <v>9.48</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="8">
         <f t="shared" si="0"/>
         <v>1.474339035769829E-2</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="5">
         <v>99.98</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="6">
         <v>34.94</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="5">
         <v>0.69</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="5">
         <v>2</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>1440</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="7">
         <v>31.07</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="8">
         <f t="shared" si="0"/>
         <v>2.1576388888888888E-2</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="5">
         <v>94.79</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="6">
         <v>12.98</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="5">
         <v>1.02</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="10">
         <v>1440</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="11">
         <v>6.28</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="12">
         <f t="shared" si="0"/>
         <v>4.3611111111111116E-3</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="9">
         <v>55.47</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="10">
         <v>2.83</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="9">
         <v>0.78</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="9">
         <v>28</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
+      <c r="Z10"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>1440</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="7">
         <v>17.5</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="8">
         <f t="shared" si="0"/>
         <v>1.2152777777777778E-2</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="5">
         <v>84.88</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="6">
         <v>35.39</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="5">
         <v>1.93</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="10">
         <v>1440</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="11">
         <v>6.32</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="12">
         <f t="shared" si="0"/>
         <v>4.3888888888888892E-3</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="9">
         <v>58.53</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="10">
         <v>3.54</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="9">
         <v>0.96</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="9">
         <v>28</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+      <c r="Y12"/>
+      <c r="Z12"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="6">
         <v>1440</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="7">
         <v>35.86</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="8">
         <f t="shared" si="0"/>
         <v>2.4902777777777777E-2</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="5">
         <v>96.76</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="6">
         <v>1571.44</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="5">
         <v>4.22</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="6">
         <v>1440</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="7">
         <v>53.81</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="8">
         <f t="shared" si="0"/>
         <v>3.7368055555555557E-2</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="5">
         <v>99.11</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="6">
         <v>18.329999999999998</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="5">
         <v>3.57</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="6">
         <v>1440</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="7">
         <v>69.180000000000007</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="8">
         <f t="shared" si="0"/>
         <v>4.804166666666667E-2</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="5">
         <v>99.82</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="6">
         <v>150.94999999999999</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="5">
         <v>2.88</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="10">
         <v>792</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="11">
         <v>2.2400000000000002</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="12">
         <f t="shared" si="0"/>
         <v>2.8282828282828287E-3</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="9">
         <v>93.74</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="10">
         <v>3.81</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="9">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="9">
         <v>58</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16"/>
+      <c r="W16"/>
+      <c r="X16"/>
+      <c r="Y16"/>
+      <c r="Z16"/>
+    </row>
+    <row r="17" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="10">
         <v>792</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="11">
         <v>6.1</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="12">
         <f t="shared" si="0"/>
         <v>7.7020202020202013E-3</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="9">
         <v>96.23</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="10">
         <v>1.65</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="9">
         <v>0.42</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="9">
         <v>57</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+      <c r="V17"/>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="Y17"/>
+      <c r="Z17"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="6">
         <v>792</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="7">
         <v>1</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="8">
         <f t="shared" si="0"/>
         <v>1.2626262626262627E-3</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="5">
         <v>88.99</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="6">
         <v>6.72</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="5">
         <v>0.46</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="5">
         <v>23</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="19" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="10">
         <v>792</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="11">
         <v>6.04</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="12">
         <f t="shared" si="0"/>
         <v>7.6262626262626259E-3</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="9">
         <v>96.15</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="10">
         <v>2.16</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="9">
         <v>0.81</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="9">
         <v>61</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19" s="9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19"/>
+      <c r="W19"/>
+      <c r="X19"/>
+      <c r="Y19"/>
+      <c r="Z19"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="6">
         <v>792</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="7">
         <v>1.84</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="8">
         <f t="shared" si="0"/>
         <v>2.3232323232323234E-3</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="5">
         <v>93.36</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="6">
         <v>202.51</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="5">
         <v>0.59</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="6">
         <v>792</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="7">
         <v>3.14</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="8">
         <f t="shared" si="0"/>
         <v>3.964646464646465E-3</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="5">
         <v>95.61</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="6">
         <v>4.34</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="5">
         <v>0.51</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="6">
         <v>792</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="7">
         <v>3.89</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="8">
         <f t="shared" si="0"/>
         <v>4.911616161616162E-3</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="5">
         <v>95.43</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="6">
         <v>31.37</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="5">
         <v>0.57999999999999996</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="5">
         <v>8</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="6">
         <v>659</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="7">
         <v>7.31</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="8">
         <f t="shared" si="0"/>
         <v>1.1092564491654021E-2</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="5">
         <v>90.7</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="6">
         <v>5.13</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="5">
         <v>0.43</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="5">
         <v>33</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="24" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="10">
         <v>659</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="11">
         <v>6.37</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="12">
         <f t="shared" si="0"/>
         <v>9.6661608497723827E-3</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="9">
         <v>88.25</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="10">
         <v>1.57</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="9">
         <v>0.43</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="9">
         <v>58</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24"/>
+      <c r="U24"/>
+      <c r="V24"/>
+      <c r="W24"/>
+      <c r="X24"/>
+      <c r="Y24"/>
+      <c r="Z24"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="6">
         <v>659</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="7">
         <v>3.21</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="8">
         <f t="shared" si="0"/>
         <v>4.871016691957511E-3</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="5">
         <v>80.92</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="6">
         <v>11.44</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="5">
         <v>0.69</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="5">
         <v>21</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="6">
         <v>659</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="7">
         <v>6.55</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="8">
         <f t="shared" si="0"/>
         <v>9.9393019726858878E-3</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="5">
         <v>88.57</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="6">
         <v>1.82</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="5">
         <v>0.76</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="5">
         <v>85</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K26" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="6">
         <v>659</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="7">
         <v>6.64</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="8">
         <f t="shared" si="0"/>
         <v>1.0075872534142639E-2</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="5">
         <v>90.48</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="6">
         <v>409.1</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="5">
         <v>1.4</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="6">
         <v>659</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="7">
         <v>7.95</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="8">
         <f t="shared" si="0"/>
         <v>1.2063732928679818E-2</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="5">
         <v>92.19</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="6">
         <v>5.61</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="5">
         <v>0.91</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="5">
         <v>1</v>
       </c>
-      <c r="K28" t="s">
+      <c r="J28" s="5"/>
+      <c r="K28" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="6">
         <v>659</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="7">
         <v>14.24</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="8">
         <f t="shared" si="0"/>
         <v>2.1608497723823977E-2</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="5">
         <v>93.89</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="6">
         <v>57.26</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="5">
         <v>1.05</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="5">
         <v>3</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J29" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K29" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="6">
         <v>1440</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="7">
         <v>9.7200000000000006</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="8">
         <f t="shared" si="0"/>
         <v>6.7500000000000008E-3</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="5">
         <v>92.45</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="6">
         <v>10.76</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="5">
         <v>0.68</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="6">
         <v>1440</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="7">
         <v>6.08</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31" s="8">
         <f t="shared" si="0"/>
         <v>4.2222222222222227E-3</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="5">
         <v>89.61</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="6">
         <v>2.6</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="5">
         <v>0.56999999999999995</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="5">
         <v>14</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K31" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A32" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="6">
         <v>1440</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="7">
         <v>2.8</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" s="8">
         <f t="shared" si="0"/>
         <v>1.9444444444444444E-3</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="5">
         <v>85.62</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="6">
         <v>11.7</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="5">
         <v>0.87</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+    </row>
+    <row r="33" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="10">
         <v>1440</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="11">
         <v>6.23</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33" s="12">
         <f t="shared" si="0"/>
         <v>4.3263888888888892E-3</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="9">
         <v>90.86</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="10">
         <v>3.57</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="9">
         <v>0.99</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="9">
         <v>26</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J33" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="K33" t="s">
+      <c r="K33" s="9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+      <c r="S33"/>
+      <c r="T33"/>
+      <c r="U33"/>
+      <c r="V33"/>
+      <c r="W33"/>
+      <c r="X33"/>
+      <c r="Y33"/>
+      <c r="Z33"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="6">
         <v>1440</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="7">
         <v>7.23</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" s="8">
         <f t="shared" si="0"/>
         <v>5.0208333333333337E-3</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="5">
         <v>91.95</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="6">
         <v>716.53</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="5">
         <v>2.16</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A35" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="6">
         <v>1440</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="7">
         <v>7.12</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="8">
         <f t="shared" si="0"/>
         <v>4.9444444444444449E-3</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="5">
         <v>93.92</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="6">
         <v>9.6300000000000008</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="5">
         <v>1.2</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="6">
         <v>1440</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="7">
         <v>30.84</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36" s="8">
         <f t="shared" si="0"/>
         <v>2.1416666666666667E-2</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="5">
         <v>94.61</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="6">
         <v>137.94</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="5">
         <v>1.95</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="6">
         <v>1080</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="7">
         <v>9.06</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" s="8">
         <f t="shared" si="0"/>
         <v>8.3888888888888902E-3</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="5">
         <v>96.78</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="6">
         <v>8.5</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="5">
         <v>0.49</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A38" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="6">
         <v>1080</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="7">
         <v>9.2200000000000006</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="8">
         <f t="shared" si="0"/>
         <v>8.5370370370370374E-3</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="5">
         <v>96.54</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="6">
         <v>2.85</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="5">
         <v>0.52</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="5">
         <v>16</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J38" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K38" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A39" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="6">
         <v>1080</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="7">
         <v>3.54</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="8">
         <f t="shared" si="0"/>
         <v>3.2777777777777779E-3</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="5">
         <v>91.07</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="6">
         <v>17.04</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="5">
         <v>0.7</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+    </row>
+    <row r="40" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="10">
         <v>1080</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="11">
         <v>9.42</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="12">
         <f t="shared" si="0"/>
         <v>8.7222222222222215E-3</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="9">
         <v>97.95</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="10">
         <v>2.75</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="9">
         <v>1.01</v>
       </c>
-      <c r="I40">
+      <c r="I40" s="9">
         <v>32</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J40" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="K40" t="s">
+      <c r="K40" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+      <c r="R40"/>
+      <c r="S40"/>
+      <c r="T40"/>
+      <c r="U40"/>
+      <c r="V40"/>
+      <c r="W40"/>
+      <c r="X40"/>
+      <c r="Y40"/>
+      <c r="Z40"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="6">
         <v>1080</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="7">
         <v>5.48</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41" s="8">
         <f t="shared" si="0"/>
         <v>5.0740740740740746E-3</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="5">
         <v>96.28</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="6">
         <v>564.87</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="5">
         <v>0.89</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A42" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="6">
         <v>1080</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="7">
         <v>6.14</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E42" s="8">
         <f t="shared" si="0"/>
         <v>5.6851851851851846E-3</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="5">
         <v>97.33</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="6">
         <v>5.71</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="5">
         <v>0.73</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="5">
         <v>1</v>
       </c>
-      <c r="K42" t="s">
+      <c r="J42" s="5"/>
+      <c r="K42" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A43" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="6">
         <v>1080</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="7">
         <v>8.9700000000000006</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E43" s="8">
         <f t="shared" si="0"/>
         <v>8.3055555555555556E-3</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="5">
         <v>98.37</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="6">
         <v>40.28</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="5">
         <v>0.64</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="5">
         <v>2</v>
       </c>
-      <c r="J43" t="s">
+      <c r="J43" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="K43" t="s">
+      <c r="K43" s="5" t="s">
         <v>16</v>
       </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A44" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="6">
+        <v>1483.16</v>
+      </c>
+      <c r="D44" s="7">
+        <v>43.16</v>
+      </c>
+      <c r="E44" s="8">
+        <v>2.91</v>
+      </c>
+      <c r="F44" s="5">
+        <v>85.31</v>
+      </c>
+      <c r="G44" s="6">
+        <v>11.52</v>
+      </c>
+      <c r="H44" s="5">
+        <v>0.94</v>
+      </c>
+      <c r="I44" s="5">
+        <v>3</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="10">
+        <v>1483.16</v>
+      </c>
+      <c r="D45" s="11">
+        <v>6.18</v>
+      </c>
+      <c r="E45" s="12">
+        <v>0.42</v>
+      </c>
+      <c r="F45" s="9">
+        <v>38.979999999999997</v>
+      </c>
+      <c r="G45" s="10">
+        <v>2.64</v>
+      </c>
+      <c r="H45" s="9">
+        <v>0.54</v>
+      </c>
+      <c r="I45" s="9">
+        <v>30</v>
+      </c>
+      <c r="J45" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="K45" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+      <c r="O45"/>
+      <c r="P45"/>
+      <c r="Q45"/>
+      <c r="R45"/>
+      <c r="S45"/>
+      <c r="T45"/>
+      <c r="U45"/>
+      <c r="V45"/>
+      <c r="W45"/>
+      <c r="X45"/>
+      <c r="Y45"/>
+      <c r="Z45"/>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="6">
+        <v>1483.16</v>
+      </c>
+      <c r="D46" s="7">
+        <v>21.66</v>
+      </c>
+      <c r="E46" s="8">
+        <v>1.46</v>
+      </c>
+      <c r="F46" s="5">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="G46" s="6">
+        <v>32.35</v>
+      </c>
+      <c r="H46" s="5">
+        <v>1.53</v>
+      </c>
+      <c r="I46" s="5">
+        <v>0</v>
+      </c>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+    </row>
+    <row r="47" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="10">
+        <v>1483.16</v>
+      </c>
+      <c r="D47" s="11">
+        <v>6.35</v>
+      </c>
+      <c r="E47" s="12">
+        <v>0.43</v>
+      </c>
+      <c r="F47" s="9">
+        <v>43.86</v>
+      </c>
+      <c r="G47" s="10">
+        <v>3.47</v>
+      </c>
+      <c r="H47" s="9">
+        <v>0.69</v>
+      </c>
+      <c r="I47" s="9">
+        <v>30</v>
+      </c>
+      <c r="J47" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="K47" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="L47"/>
+      <c r="M47"/>
+      <c r="N47"/>
+      <c r="O47"/>
+      <c r="P47"/>
+      <c r="Q47"/>
+      <c r="R47"/>
+      <c r="S47"/>
+      <c r="T47"/>
+      <c r="U47"/>
+      <c r="V47"/>
+      <c r="W47"/>
+      <c r="X47"/>
+      <c r="Y47"/>
+      <c r="Z47"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="6">
+        <v>1483.16</v>
+      </c>
+      <c r="D48" s="7">
+        <v>58.51</v>
+      </c>
+      <c r="E48" s="8">
+        <v>3.95</v>
+      </c>
+      <c r="F48" s="5">
+        <v>89.65</v>
+      </c>
+      <c r="G48" s="6">
+        <v>1330.9</v>
+      </c>
+      <c r="H48" s="5">
+        <v>3.75</v>
+      </c>
+      <c r="I48" s="5">
+        <v>0</v>
+      </c>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A49" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" s="6">
+        <v>1483.16</v>
+      </c>
+      <c r="D49" s="7">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="E49" s="8">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="F49" s="5">
+        <v>94.82</v>
+      </c>
+      <c r="G49" s="6">
+        <v>13.12</v>
+      </c>
+      <c r="H49" s="5">
+        <v>4.18</v>
+      </c>
+      <c r="I49" s="5">
+        <v>1</v>
+      </c>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A50" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="6">
+        <v>1483.16</v>
+      </c>
+      <c r="D50" s="7">
+        <v>126.97</v>
+      </c>
+      <c r="E50" s="8">
+        <v>8.56</v>
+      </c>
+      <c r="F50" s="5">
+        <v>97.52</v>
+      </c>
+      <c r="G50" s="6">
+        <v>181.25</v>
+      </c>
+      <c r="H50" s="5">
+        <v>2.88</v>
+      </c>
+      <c r="I50" s="5">
+        <v>0</v>
+      </c>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>